<commit_message>
Update XLS file with first tests in lab Fix GrayToTime algo
</commit_message>
<xml_diff>
--- a/GrayToTime/GrayToTime.xlsx
+++ b/GrayToTime/GrayToTime.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivier.vanhoucke\Desktop\VMShare\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivier.vanhoucke\Desktop\VMShare\Debug\GrayToTime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8C1DCB-B85B-4F9B-AADE-5B76BE870C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8477C992-15CC-4E5F-A6EB-F1911B0CBA43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -395,8 +395,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:trendlineType val="log"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -404,6 +403,336 @@
                 <c:manualLayout>
                   <c:x val="0.10401771653543307"/>
                   <c:y val="-0.51612715077282001"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.12959042444980265"/>
+                  <c:y val="-0.54167484604590632"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.5589917524604218E-2"/>
+                  <c:y val="-0.79143237289244661"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.14520255330218404"/>
+                  <c:y val="-0.65289331908303705"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="4"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="4"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.1964335144256905E-2"/>
+                  <c:y val="-0.57511251190554091"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -446,7 +775,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>50</c:v>
@@ -473,25 +802,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>800</c:v>
+                  <c:v>90000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>600</c:v>
+                  <c:v>72000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>400</c:v>
+                  <c:v>31000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>200</c:v>
+                  <c:v>15000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>80</c:v>
+                  <c:v>12500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80</c:v>
+                  <c:v>9500</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80</c:v>
+                  <c:v>8500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1250,16 +1579,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>518160</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1553,7 +1882,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1579,11 +1908,11 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>800</v>
+        <v>90000</v>
       </c>
       <c r="C2" s="3">
-        <f>IF(B2&gt;$C$11,$C$11,IF(B2&lt;$B$11,$B$11,B2))</f>
-        <v>800</v>
+        <f t="shared" ref="C2:C8" si="0">IF(B2&gt;$C$11,$C$11,IF(B2&lt;$B$11,$B$11,B2))</f>
+        <v>90000</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -1591,14 +1920,14 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2">
-        <v>600</v>
+        <v>72000</v>
       </c>
       <c r="C3" s="3">
-        <f t="shared" ref="C3:C8" si="0">IF(B3&gt;$C$11,$C$11,IF(B3&lt;$B$11,$B$11,B3))</f>
-        <v>600</v>
+        <f t="shared" si="0"/>
+        <v>72000</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -1609,11 +1938,11 @@
         <v>50</v>
       </c>
       <c r="B4" s="2">
-        <v>400</v>
+        <v>31000</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>31000</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -1624,11 +1953,11 @@
         <v>100</v>
       </c>
       <c r="B5" s="2">
-        <v>200</v>
+        <v>15000</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>15000</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
@@ -1639,11 +1968,11 @@
         <v>150</v>
       </c>
       <c r="B6" s="2">
-        <v>50</v>
+        <v>12500</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>12500</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
@@ -1654,11 +1983,11 @@
         <v>200</v>
       </c>
       <c r="B7" s="2">
-        <v>5</v>
+        <v>9500</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>9500</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
@@ -1669,11 +1998,11 @@
         <v>255</v>
       </c>
       <c r="B8" s="2">
-        <v>0</v>
+        <v>8500</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>8500</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
@@ -1692,10 +2021,10 @@
         <v>0</v>
       </c>
       <c r="B11" s="2">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="C11" s="2">
-        <v>3000</v>
+        <v>90000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add sensor calculation add picture fix exception when port is deconnected update TODO
</commit_message>
<xml_diff>
--- a/GrayToTime/GrayToTime.xlsx
+++ b/GrayToTime/GrayToTime.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivier.vanhoucke\Desktop\VMShare\Debug\GrayToTime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8477C992-15CC-4E5F-A6EB-F1911B0CBA43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085032DC-1947-45A2-B24D-760514141FD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GrayToTime" sheetId="1" r:id="rId1"/>
+    <sheet name="GrayToTime (sensor)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
   <si>
     <t>Duration</t>
   </si>
@@ -131,11 +132,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calcul" xfId="2" builtinId="22"/>
@@ -1019,7 +1021,509 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>GrayToTime (sensor)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.5481479870264833E-2"/>
+                  <c:y val="-0.60031618711212498"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'GrayToTime (sensor)'!$C$4:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>238</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'GrayToTime (sensor)'!$B$4:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>34000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>36000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>38000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>40000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000011-6FF8-4043-93F9-65CF3F02D38C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="307797728"/>
+        <c:axId val="368881904"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="307797728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="368881904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="368881904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="307797728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1575,6 +2079,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1600,6 +2620,49 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81184B7B-44BB-4631-AA9F-931AA80E3C0E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1881,8 +2944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2032,4 +3095,285 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77C416AC-F0E5-4357-878E-3E573384E3D8}">
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>40000</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3">
+        <f>A4*$A$2/MAX(A4:A23)</f>
+        <v>2000</v>
+      </c>
+      <c r="C4" s="4">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3">
+        <f t="shared" ref="B5:B23" si="0">A5*$A$2/MAX(A5:A24)</f>
+        <v>4000</v>
+      </c>
+      <c r="C5" s="4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+      <c r="C6" s="4">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3">
+        <f t="shared" si="0"/>
+        <v>8000</v>
+      </c>
+      <c r="C7" s="4">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3">
+        <f t="shared" si="0"/>
+        <v>10000</v>
+      </c>
+      <c r="C8" s="4">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3">
+        <f t="shared" si="0"/>
+        <v>12000</v>
+      </c>
+      <c r="C9" s="4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3">
+        <f t="shared" si="0"/>
+        <v>14000</v>
+      </c>
+      <c r="C10" s="4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3">
+        <f t="shared" si="0"/>
+        <v>16000</v>
+      </c>
+      <c r="C11" s="4">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3">
+        <f t="shared" si="0"/>
+        <v>18000</v>
+      </c>
+      <c r="C12" s="4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+      <c r="C13" s="4">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
+        <v>22000</v>
+      </c>
+      <c r="C14" s="4">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" si="0"/>
+        <v>24000</v>
+      </c>
+      <c r="C15" s="4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" si="0"/>
+        <v>26000</v>
+      </c>
+      <c r="C16" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" s="3">
+        <f t="shared" si="0"/>
+        <v>28000</v>
+      </c>
+      <c r="C17" s="4">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" s="3">
+        <f t="shared" si="0"/>
+        <v>30000</v>
+      </c>
+      <c r="C18" s="4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" s="3">
+        <f t="shared" si="0"/>
+        <v>32000</v>
+      </c>
+      <c r="C19" s="4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" s="3">
+        <f t="shared" si="0"/>
+        <v>34000</v>
+      </c>
+      <c r="C20" s="4">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3">
+        <f t="shared" si="0"/>
+        <v>36000</v>
+      </c>
+      <c r="C21" s="4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" s="3">
+        <f t="shared" si="0"/>
+        <v>38000</v>
+      </c>
+      <c r="C22" s="4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" s="3">
+        <f t="shared" si="0"/>
+        <v>40000</v>
+      </c>
+      <c r="C23" s="4">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>